<commit_message>
Correction coef Grille sTI2D
</commit_message>
<xml_diff>
--- a/tables/Grille_presentation_projet_STI2D_V2015.xlsx
+++ b/tables/Grille_presentation_projet_STI2D_V2015.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="-15" windowWidth="10200" windowHeight="7575" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="-15" windowWidth="14445" windowHeight="12165" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="125725" calcOnSave="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1276,6 +1276,129 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1297,34 +1420,15 @@
     <xf numFmtId="0" fontId="30" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1332,72 +1436,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1405,44 +1443,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1515,26 +1515,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="104157184"/>
-        <c:axId val="104158720"/>
+        <c:axId val="90128384"/>
+        <c:axId val="90129920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104157184"/>
+        <c:axId val="90128384"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104158720"/>
+        <c:crossAx val="90129920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104158720"/>
+        <c:axId val="90129920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1545,7 +1544,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104157184"/>
+        <c:crossAx val="90128384"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1561,7 +1560,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1605,26 +1604,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="104178432"/>
-        <c:axId val="104179968"/>
+        <c:axId val="90149632"/>
+        <c:axId val="90151168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104178432"/>
+        <c:axId val="90149632"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104179968"/>
+        <c:crossAx val="90151168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104179968"/>
+        <c:axId val="90151168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1635,7 +1633,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104178432"/>
+        <c:crossAx val="90149632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1651,7 +1649,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1692,26 +1690,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="104199680"/>
-        <c:axId val="104201216"/>
+        <c:axId val="90170880"/>
+        <c:axId val="90172416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104199680"/>
+        <c:axId val="90170880"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104201216"/>
+        <c:crossAx val="90172416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104201216"/>
+        <c:axId val="90172416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1722,7 +1719,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104199680"/>
+        <c:crossAx val="90170880"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1738,7 +1735,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1773,26 +1770,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="104499456"/>
-        <c:axId val="104501248"/>
+        <c:axId val="94267648"/>
+        <c:axId val="94273536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104499456"/>
+        <c:axId val="94267648"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104501248"/>
+        <c:crossAx val="94273536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104501248"/>
+        <c:axId val="94273536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1803,7 +1799,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="104499456"/>
+        <c:crossAx val="94267648"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1819,7 +1815,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2283,8 +2279,8 @@
   </sheetPr>
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75"/>
@@ -2321,10 +2317,10 @@
       <c r="H1" s="26"/>
       <c r="I1" s="56"/>
       <c r="J1" s="57"/>
-      <c r="K1" s="112" t="s">
+      <c r="K1" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="113"/>
+      <c r="L1" s="109"/>
       <c r="M1" s="60"/>
       <c r="N1" s="61"/>
     </row>
@@ -2332,11 +2328,11 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="J2" s="58" t="s">
         <v>0</v>
       </c>
@@ -2355,10 +2351,10 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="121"/>
+      <c r="B3" s="117"/>
       <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
@@ -2395,16 +2391,16 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="124"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="120"/>
       <c r="I4" s="16"/>
       <c r="J4" s="46">
         <v>0.2</v>
@@ -2430,13 +2426,13 @@
       <c r="A5" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="121" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="99"/>
+      <c r="D5" s="122"/>
       <c r="E5" s="81"/>
       <c r="F5" s="81"/>
       <c r="G5" s="81"/>
@@ -2448,7 +2444,7 @@
       <c r="J5" s="68">
         <v>1</v>
       </c>
-      <c r="L5" s="135">
+      <c r="L5" s="92">
         <f>SUM(N5:N6)</f>
         <v>0</v>
       </c>
@@ -2481,11 +2477,11 @@
     </row>
     <row r="6" spans="1:26" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="104"/>
-      <c r="B6" s="105"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="101"/>
+      <c r="D6" s="123"/>
       <c r="E6" s="31"/>
       <c r="F6" s="82"/>
       <c r="G6" s="82"/>
@@ -2497,7 +2493,7 @@
       <c r="J6" s="68">
         <v>1</v>
       </c>
-      <c r="L6" s="136"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="71">
         <f>1</f>
         <v>1</v>
@@ -2535,7 +2531,7 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="101"/>
+      <c r="D7" s="123"/>
       <c r="E7" s="62"/>
       <c r="F7" s="62"/>
       <c r="G7" s="62"/>
@@ -2579,16 +2575,16 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="119"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="115"/>
       <c r="I8" s="16"/>
       <c r="J8" s="46">
         <v>0.15</v>
@@ -2622,7 +2618,7 @@
       <c r="C9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="99"/>
+      <c r="D9" s="122"/>
       <c r="E9" s="34"/>
       <c r="F9" s="83"/>
       <c r="G9" s="80"/>
@@ -2634,7 +2630,7 @@
       <c r="J9" s="68">
         <v>1</v>
       </c>
-      <c r="L9" s="135">
+      <c r="L9" s="92">
         <f>SUM(N9:N11)</f>
         <v>0</v>
       </c>
@@ -2671,7 +2667,7 @@
       <c r="C10" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="100"/>
+      <c r="D10" s="139"/>
       <c r="E10" s="64"/>
       <c r="F10" s="84"/>
       <c r="G10" s="90"/>
@@ -2683,7 +2679,7 @@
       <c r="J10" s="68">
         <v>1</v>
       </c>
-      <c r="L10" s="137"/>
+      <c r="L10" s="94"/>
       <c r="M10" s="71">
         <f>1</f>
         <v>1</v>
@@ -2717,7 +2713,7 @@
       <c r="C11" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="101"/>
+      <c r="D11" s="123"/>
       <c r="E11" s="66"/>
       <c r="F11" s="85"/>
       <c r="G11" s="91"/>
@@ -2729,7 +2725,7 @@
       <c r="J11" s="68">
         <v>1</v>
       </c>
-      <c r="L11" s="136"/>
+      <c r="L11" s="93"/>
       <c r="M11" s="71">
         <f>1</f>
         <v>1</v>
@@ -2761,13 +2757,13 @@
       <c r="A12" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="121" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="101"/>
+      <c r="D12" s="123"/>
       <c r="E12" s="36"/>
       <c r="F12" s="86"/>
       <c r="G12" s="86"/>
@@ -2779,7 +2775,7 @@
       <c r="J12" s="68">
         <v>1</v>
       </c>
-      <c r="L12" s="135">
+      <c r="L12" s="92">
         <f>SUM(N12:N13)</f>
         <v>0</v>
       </c>
@@ -2811,12 +2807,12 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="106"/>
-      <c r="B13" s="107"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="102"/>
+      <c r="D13" s="140"/>
       <c r="E13" s="38"/>
       <c r="F13" s="87"/>
       <c r="G13" s="87"/>
@@ -2828,7 +2824,7 @@
       <c r="J13" s="68">
         <v>1</v>
       </c>
-      <c r="L13" s="136"/>
+      <c r="L13" s="93"/>
       <c r="M13" s="71">
         <f>1</f>
         <v>1</v>
@@ -2857,16 +2853,16 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="98"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="137"/>
+      <c r="G14" s="137"/>
+      <c r="H14" s="138"/>
       <c r="I14" s="16"/>
       <c r="J14" s="46">
         <v>0.45</v>
@@ -2900,7 +2896,7 @@
       <c r="C15" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="99"/>
+      <c r="D15" s="122"/>
       <c r="E15" s="36"/>
       <c r="F15" s="86"/>
       <c r="G15" s="86"/>
@@ -2953,7 +2949,7 @@
       <c r="C16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="101"/>
+      <c r="D16" s="123"/>
       <c r="E16" s="34"/>
       <c r="F16" s="83"/>
       <c r="G16" s="83"/>
@@ -3000,13 +2996,13 @@
       <c r="A17" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="121" t="s">
         <v>30</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="101"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="65"/>
       <c r="F17" s="88"/>
       <c r="G17" s="88"/>
@@ -3018,7 +3014,7 @@
       <c r="J17" s="68">
         <v>1</v>
       </c>
-      <c r="L17" s="135">
+      <c r="L17" s="92">
         <f>SUM(N17:N18)</f>
         <v>0</v>
       </c>
@@ -3050,12 +3046,12 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A18" s="106"/>
-      <c r="B18" s="107"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="103"/>
+      <c r="D18" s="141"/>
       <c r="E18" s="67"/>
       <c r="F18" s="89"/>
       <c r="G18" s="89"/>
@@ -3067,7 +3063,7 @@
       <c r="J18" s="68">
         <v>1</v>
       </c>
-      <c r="L18" s="136"/>
+      <c r="L18" s="93"/>
       <c r="M18" s="71">
         <f>1</f>
         <v>1</v>
@@ -3096,16 +3092,16 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="96" t="s">
+      <c r="A19" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="98"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="138"/>
       <c r="I19" s="16"/>
       <c r="J19" s="46">
         <v>0.2</v>
@@ -3133,13 +3129,13 @@
       <c r="A20" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="105" t="s">
+      <c r="B20" s="121" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="99"/>
+      <c r="D20" s="122"/>
       <c r="E20" s="36"/>
       <c r="F20" s="86"/>
       <c r="G20" s="86"/>
@@ -3149,7 +3145,7 @@
         <v>◄</v>
       </c>
       <c r="J20" s="68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" s="48">
         <f>SUM(N20)</f>
@@ -3184,11 +3180,11 @@
     </row>
     <row r="21" spans="1:26" ht="14.1" customHeight="1">
       <c r="A21" s="104"/>
-      <c r="B21" s="105"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="101"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="34"/>
       <c r="F21" s="83"/>
       <c r="G21" s="83"/>
@@ -3233,10 +3229,10 @@
     </row>
     <row r="22" spans="1:26">
       <c r="C22" s="17"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
       <c r="J22" s="19">
         <f>J4+J8+J19+J14</f>
         <v>1</v>
@@ -3262,15 +3258,15 @@
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="114">
+      <c r="E23" s="110">
         <f>IF(M22&lt;&gt;1,"",L4+L8+L14+L19)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="114"/>
-      <c r="G23" s="115" t="s">
+      <c r="F23" s="110"/>
+      <c r="G23" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="115"/>
+      <c r="H23" s="111"/>
       <c r="I23" s="20"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -3289,12 +3285,12 @@
       <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="139"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="141" t="s">
+      <c r="E24" s="96"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="142"/>
+      <c r="H24" s="99"/>
       <c r="K24" s="125" t="s">
         <v>49</v>
       </c>
@@ -3316,15 +3312,15 @@
       <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="143">
+      <c r="E25" s="100">
         <f>E24*6</f>
         <v>0</v>
       </c>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145">
+      <c r="F25" s="101"/>
+      <c r="G25" s="102">
         <v>120</v>
       </c>
-      <c r="H25" s="146"/>
+      <c r="H25" s="103"/>
       <c r="I25" s="16"/>
       <c r="K25" s="127"/>
       <c r="L25" s="128"/>
@@ -3342,14 +3338,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="138"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="138"/>
+      <c r="A26" s="95"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -3395,14 +3391,14 @@
         <v>46</v>
       </c>
       <c r="B28" s="130"/>
-      <c r="C28" s="132" t="s">
+      <c r="C28" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="134"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="146"/>
       <c r="I28" s="22"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3418,14 +3414,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="27.95" customHeight="1">
-      <c r="A29" s="94"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="108"/>
+      <c r="A29" s="134"/>
+      <c r="B29" s="135"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="135"/>
+      <c r="H29" s="142"/>
       <c r="I29" s="23"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -3441,14 +3437,14 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="27.95" customHeight="1" thickBot="1">
-      <c r="A30" s="94"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="108"/>
+      <c r="A30" s="134"/>
+      <c r="B30" s="135"/>
+      <c r="C30" s="135"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="135"/>
+      <c r="H30" s="142"/>
       <c r="I30" s="23"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -3468,20 +3464,20 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="27.95" customHeight="1" thickBot="1">
-      <c r="A31" s="92"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="109"/>
+      <c r="A31" s="132"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="143"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="110" t="s">
+      <c r="K31" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="L31" s="111"/>
+      <c r="L31" s="107"/>
       <c r="N31" s="49"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -3647,16 +3643,22 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C29:H31"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A27:H27"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="E23:F23"/>
@@ -3673,22 +3675,16 @@
     <mergeCell ref="K24:L25"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C29:H31"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>